<commit_message>
made changes proposed by SonarLint
</commit_message>
<xml_diff>
--- a/cmir3097/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/cmir3097/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ralub\Downloads\CheckLists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facultate\an_3\sem2\vvss\lab\3Testeri\cmir3097\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60358929-C9CB-4EB6-A638-A2AF2AD3D5A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556F7E59-700A-4455-B494-7A45B4E70686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="108">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -282,6 +282,85 @@
   </si>
   <si>
     <t>Comanciu Maria-Cristina</t>
+  </si>
+  <si>
+    <t>Task, line 125</t>
+  </si>
+  <si>
+    <t>Refactor nextTimeAfter method to reduce its Cognitive Complexity</t>
+  </si>
+  <si>
+    <t>Codul este ingramadit si greu de inteles</t>
+  </si>
+  <si>
+    <t>Am creat metode noi care au fiecare propriul rol.</t>
+  </si>
+  <si>
+    <t>Task, line 233</t>
+  </si>
+  <si>
+    <t>Remove this "clone"  impl</t>
+  </si>
+  <si>
+    <t>Use the opposite operator "!="</t>
+  </si>
+  <si>
+    <t>!(this.interval == 0)</t>
+  </si>
+  <si>
+    <t>this.interval != 0</t>
+  </si>
+  <si>
+    <t>Am adaugat un constructor care are ca parametru un obiect de tip task si salveaza atributele acestuia</t>
+  </si>
+  <si>
+    <t>Task, line 146, 150</t>
+  </si>
+  <si>
+    <t>Remove unused method parameter "current"</t>
+  </si>
+  <si>
+    <t>current este parametru la cele 2 functii</t>
+  </si>
+  <si>
+    <t>l-am eliminat ca parametru</t>
+  </si>
+  <si>
+    <t>Make "sdf" an instance variable</t>
+  </si>
+  <si>
+    <t>eliminarea keyword ului static duce la erori in teste</t>
+  </si>
+  <si>
+    <t>private static final SimpleDateFormat sdf</t>
+  </si>
+  <si>
+    <t>Task, line 13</t>
+  </si>
+  <si>
+    <t>TaskList, line 36</t>
+  </si>
+  <si>
+    <t>Replace sout by a logger</t>
+  </si>
+  <si>
+    <t>System.out.println(getTask(i).getTitle());</t>
+  </si>
+  <si>
+    <t>logger.info(getTask(i).getTitle());</t>
+  </si>
+  <si>
+    <t>TaskList, line 21</t>
+  </si>
+  <si>
+    <t>"Iterator" is defined int the "Iterable" interafce and can be removed from this class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+   public abstract Iterator&lt;Task&gt; iterator();</t>
+  </si>
+  <si>
+    <t>am eliminat aceasta linie de cod</t>
   </si>
 </sst>
 </file>
@@ -863,19 +942,19 @@
       <selection activeCell="D6" sqref="D6:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.90625" style="6"/>
+    <col min="2" max="2" width="12.36328125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.36328125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.90625" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="6"/>
+    <col min="10" max="10" width="14.453125" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.90625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -886,7 +965,7 @@
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B2" s="26" t="s">
         <v>16</v>
       </c>
@@ -901,7 +980,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H3" s="17" t="s">
         <v>17</v>
       </c>
@@ -912,7 +991,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
@@ -930,7 +1009,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
@@ -948,7 +1027,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -956,14 +1035,14 @@
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -977,7 +1056,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -991,7 +1070,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1006,7 +1085,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -1021,7 +1100,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1036,7 +1115,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1051,7 +1130,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1066,7 +1145,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1081,7 +1160,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1096,7 +1175,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1105,7 +1184,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1114,7 +1193,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1123,7 +1202,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1132,7 +1211,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1141,7 +1220,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1150,7 +1229,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1159,7 +1238,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1168,7 +1247,7 @@
       <c r="D25" s="3"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
@@ -1202,18 +1281,18 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.90625" style="6"/>
+    <col min="2" max="2" width="12.36328125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.36328125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.90625" style="6"/>
     <col min="9" max="9" width="22" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="6"/>
+    <col min="10" max="16384" width="8.90625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1224,7 +1303,7 @@
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B2" s="26" t="s">
         <v>15</v>
       </c>
@@ -1239,7 +1318,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H3" s="17" t="s">
         <v>17</v>
       </c>
@@ -1250,7 +1329,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1268,7 +1347,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
@@ -1286,7 +1365,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -1294,14 +1373,14 @@
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1315,7 +1394,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1329,7 +1408,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1344,7 +1423,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1359,7 +1438,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1374,7 +1453,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1389,7 +1468,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1402,7 +1481,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1411,7 +1490,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1420,7 +1499,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1429,7 +1508,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1438,7 +1517,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1447,7 +1526,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1456,7 +1535,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1465,7 +1544,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1474,7 +1553,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1483,7 +1562,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1492,7 +1571,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1501,7 +1580,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
@@ -1535,19 +1614,19 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" style="6"/>
+    <col min="2" max="2" width="12.36328125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="6"/>
-    <col min="9" max="9" width="26.77734375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="6"/>
+    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.90625" style="6"/>
+    <col min="9" max="9" width="26.81640625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.90625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1558,7 +1637,7 @@
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B2" s="26" t="s">
         <v>14</v>
       </c>
@@ -1573,7 +1652,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H3" s="17" t="s">
         <v>17</v>
       </c>
@@ -1584,7 +1663,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
@@ -1602,7 +1681,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
@@ -1620,7 +1699,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -1628,14 +1707,14 @@
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1649,7 +1728,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1663,7 +1742,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1678,7 +1757,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1693,7 +1772,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1708,7 +1787,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1717,7 +1796,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1726,7 +1805,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1735,7 +1814,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1744,7 +1823,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1753,7 +1832,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1762,7 +1841,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1771,7 +1850,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1780,7 +1859,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1789,7 +1868,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1798,7 +1877,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1807,7 +1886,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1816,7 +1895,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1825,7 +1904,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1834,7 +1913,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1843,7 +1922,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1852,7 +1931,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1861,7 +1940,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
@@ -1891,24 +1970,24 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" style="6"/>
+    <col min="2" max="2" width="12.36328125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="24.7265625" style="6" customWidth="1"/>
     <col min="5" max="5" width="24" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.88671875" style="6"/>
-    <col min="9" max="9" width="26.77734375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="6"/>
+    <col min="6" max="6" width="24.81640625" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.90625" style="6"/>
+    <col min="9" max="9" width="26.81640625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.90625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1919,7 +1998,7 @@
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B2" s="26" t="s">
         <v>27</v>
       </c>
@@ -1934,7 +2013,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H3" s="17" t="s">
         <v>17</v>
       </c>
@@ -1945,7 +2024,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C4" s="16" t="s">
         <v>21</v>
       </c>
@@ -1961,11 +2040,13 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="23"/>
+      <c r="D5" s="23" t="s">
+        <v>63</v>
+      </c>
       <c r="E5" s="23"/>
       <c r="H5" s="17" t="s">
         <v>19</v>
@@ -1977,7 +2058,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
@@ -1986,7 +2067,7 @@
       <c r="E6" s="23"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -2003,76 +2084,130 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="77" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F11" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C14" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2082,7 +2217,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2092,7 +2227,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2102,7 +2237,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2112,7 +2247,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2122,7 +2257,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2132,7 +2267,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2142,7 +2277,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2152,7 +2287,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2162,7 +2297,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2172,7 +2307,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2182,7 +2317,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2192,7 +2327,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2202,7 +2337,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2212,7 +2347,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C32" s="36" t="s">
         <v>28</v>
       </c>

</xml_diff>